<commit_message>
case2 add 3,5 dof
</commit_message>
<xml_diff>
--- a/dynamics/src/dynamics/xlsx/task_point_3dof.xlsx
+++ b/dynamics/src/dynamics/xlsx/task_point_3dof.xlsx
@@ -423,112 +423,112 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="n">
-        <v>0.101</v>
+        <v>0.282</v>
       </c>
       <c r="B1" t="n">
-        <v>-0.249</v>
+        <v>0.139</v>
       </c>
       <c r="C1" t="n">
-        <v>0.442</v>
+        <v>-0.013</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>-0.258</v>
+        <v>0.076</v>
       </c>
       <c r="B2" t="n">
-        <v>-0.168</v>
+        <v>0.018</v>
       </c>
       <c r="C2" t="n">
-        <v>0.165</v>
+        <v>-0.075</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>-0.126</v>
+        <v>0.029</v>
       </c>
       <c r="B3" t="n">
-        <v>0.226</v>
+        <v>-0.08400000000000001</v>
       </c>
       <c r="C3" t="n">
-        <v>0.419</v>
+        <v>-0.239</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>0.068</v>
+        <v>0.073</v>
       </c>
       <c r="B4" t="n">
-        <v>0.059</v>
+        <v>0.322</v>
       </c>
       <c r="C4" t="n">
-        <v>0.225</v>
+        <v>-0.079</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>0.058</v>
+        <v>0.173</v>
       </c>
       <c r="B5" t="n">
-        <v>0.308</v>
+        <v>0.039</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.054</v>
+        <v>-0.081</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>0.039</v>
+        <v>0.065</v>
       </c>
       <c r="B6" t="n">
-        <v>0.039</v>
+        <v>0.016</v>
       </c>
       <c r="C6" t="n">
-        <v>0.386</v>
+        <v>-0.05</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>-0.362</v>
+        <v>-0.004</v>
       </c>
       <c r="B7" t="n">
-        <v>0.135</v>
+        <v>-0.042</v>
       </c>
       <c r="C7" t="n">
-        <v>0.062</v>
+        <v>0.599</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>0.008999999999999999</v>
+        <v>-0.093</v>
       </c>
       <c r="B8" t="n">
-        <v>0.046</v>
+        <v>0.298</v>
       </c>
       <c r="C8" t="n">
-        <v>0.096</v>
+        <v>0.143</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>-0.031</v>
+        <v>-0.107</v>
       </c>
       <c r="B9" t="n">
-        <v>-0</v>
+        <v>-0.387</v>
       </c>
       <c r="C9" t="n">
-        <v>0.11</v>
+        <v>0.029</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>0.37</v>
+        <v>-0.157</v>
       </c>
       <c r="B10" t="n">
-        <v>0.016</v>
+        <v>-0.185</v>
       </c>
       <c r="C10" t="n">
-        <v>0.281</v>
+        <v>-0.014</v>
       </c>
     </row>
   </sheetData>

</xml_diff>